<commit_message>
BEACH data, Feb. 5, 2018
</commit_message>
<xml_diff>
--- a/Data/Lab-linked/NitrogenIRMS.xlsx
+++ b/Data/Lab-linked/NitrogenIRMS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DayTightChunks/Documents/PhD/HydrologicalMonitoring/Data/Lab-linked/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="6165"/>
+    <workbookView xWindow="4620" yWindow="1340" windowWidth="21500" windowHeight="14180"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -13,9 +18,15 @@
   <externalReferences>
     <externalReference r:id="rId3"/>
   </externalReferences>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -339,7 +350,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -357,10 +368,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1563960714588096"/>
-          <c:y val="0.10979173639709001"/>
-          <c:w val="0.66648158496316989"/>
-          <c:h val="0.70963948710729141"/>
+          <c:x val="0.15639607145881"/>
+          <c:y val="0.10979173639709"/>
+          <c:w val="0.66648158496317"/>
+          <c:h val="0.709639487107291"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -407,160 +418,160 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="52"/>
                 <c:pt idx="0">
-                  <c:v>711</c:v>
+                  <c:v>711.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>838</c:v>
+                  <c:v>838.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>725</c:v>
+                  <c:v>725.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>392</c:v>
+                  <c:v>392.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>246</c:v>
+                  <c:v>246.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>353</c:v>
+                  <c:v>353.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>388</c:v>
+                  <c:v>388.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>453</c:v>
+                  <c:v>453.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>510</c:v>
+                  <c:v>510.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>557</c:v>
+                  <c:v>557.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>221</c:v>
+                  <c:v>221.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>297</c:v>
+                  <c:v>297.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>427</c:v>
+                  <c:v>427.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>426</c:v>
+                  <c:v>426.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>393</c:v>
+                  <c:v>393.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>558</c:v>
+                  <c:v>558.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>495</c:v>
+                  <c:v>495.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>240</c:v>
+                  <c:v>240.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>478</c:v>
+                  <c:v>478.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>778</c:v>
+                  <c:v>778.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>614</c:v>
+                  <c:v>614.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>644</c:v>
+                  <c:v>644.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>444</c:v>
+                  <c:v>444.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>215</c:v>
+                  <c:v>215.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>290</c:v>
+                  <c:v>290.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>639</c:v>
+                  <c:v>639.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>579</c:v>
+                  <c:v>579.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>502</c:v>
+                  <c:v>502.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>160</c:v>
+                  <c:v>160.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>124</c:v>
+                  <c:v>124.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>131</c:v>
+                  <c:v>131.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>121</c:v>
+                  <c:v>121.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>142</c:v>
+                  <c:v>142.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>689</c:v>
+                  <c:v>689.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>635</c:v>
+                  <c:v>635.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>471</c:v>
+                  <c:v>471.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>293</c:v>
+                  <c:v>293.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>663</c:v>
+                  <c:v>663.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>586</c:v>
+                  <c:v>586.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>371</c:v>
+                  <c:v>371.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>284</c:v>
+                  <c:v>284.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>412</c:v>
+                  <c:v>412.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>148</c:v>
+                  <c:v>148.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>167</c:v>
+                  <c:v>167.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>292</c:v>
+                  <c:v>292.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>504</c:v>
+                  <c:v>504.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>347</c:v>
+                  <c:v>347.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>278</c:v>
+                  <c:v>278.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>449</c:v>
+                  <c:v>449.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>359</c:v>
+                  <c:v>359.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>338</c:v>
+                  <c:v>338.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>349</c:v>
+                  <c:v>349.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,115 +589,115 @@
                   <c:v>-0.223</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.30299999999999999</c:v>
+                  <c:v>-0.303</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.30199999999999999</c:v>
+                  <c:v>-0.302</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-0.185</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-5.3999999999999999E-2</c:v>
+                  <c:v>-0.054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.28999999999999998</c:v>
+                  <c:v>0.29</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>-0.51</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-0.33600000000000002</c:v>
+                  <c:v>-0.336</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-4.9000000000000002E-2</c:v>
+                  <c:v>-0.049</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.175</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.0369999999999999</c:v>
+                  <c:v>1.037</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.32800000000000001</c:v>
+                  <c:v>0.328</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.91700000000000004</c:v>
+                  <c:v>0.917</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.81100000000000005</c:v>
+                  <c:v>0.811</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.60499999999999998</c:v>
+                  <c:v>0.605</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.0089999999999999</c:v>
+                  <c:v>1.009</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>1.389</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.47899999999999998</c:v>
+                  <c:v>0.479</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.41499999999999998</c:v>
+                  <c:v>0.415</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-0.26400000000000001</c:v>
+                  <c:v>-0.264</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.69399999999999995</c:v>
+                  <c:v>0.694</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.3939999999999999</c:v>
+                  <c:v>1.394</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>1.512</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.81699999999999995</c:v>
+                  <c:v>0.817</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.35799999999999998</c:v>
+                  <c:v>0.358</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-0.16300000000000001</c:v>
+                  <c:v>-0.163</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-0.47699999999999998</c:v>
+                  <c:v>-0.477</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-0.24199999999999999</c:v>
+                  <c:v>-0.242</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>-0.98</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.51500000000000001</c:v>
+                  <c:v>0.515</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.52200000000000002</c:v>
+                  <c:v>0.522</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.6299999999999998E-2</c:v>
+                  <c:v>0.0663</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>0.627</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.44700000000000001</c:v>
+                  <c:v>0.447</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.0840000000000001</c:v>
+                  <c:v>1.084</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.97799999999999998</c:v>
+                  <c:v>0.978</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>-0.191</c:v>
@@ -698,7 +709,7 @@
                   <c:v>0.245</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-6.9000000000000006E-2</c:v>
+                  <c:v>-0.069</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>-0.125</c:v>
@@ -710,7 +721,7 @@
                   <c:v>1.028</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.0000000000000001E-3</c:v>
+                  <c:v>0.007</c:v>
                 </c:pt>
                 <c:pt idx="47">
                   <c:v>0.316</c:v>
@@ -719,13 +730,13 @@
                   <c:v>1.244</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.98899999999999999</c:v>
+                  <c:v>0.989</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.75600000000000001</c:v>
+                  <c:v>0.756</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.4339999999999999</c:v>
+                  <c:v>1.434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -754,10 +765,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -802,10 +813,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -842,6 +853,9 @@
           </c:marker>
           <c:dPt>
             <c:idx val="1"/>
+            <c:marker>
+              <c:symbol val="none"/>
+            </c:marker>
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:ln w="25400" cap="rnd">
@@ -861,10 +875,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1000</c:v>
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -876,10 +890,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-4.9999999999999989E-2</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.9999999999999989E-2</c:v>
+                  <c:v>-0.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -894,15 +908,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="156949888"/>
-        <c:axId val="158078464"/>
+        <c:axId val="738066160"/>
+        <c:axId val="738071568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="156949888"/>
+        <c:axId val="738066160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000"/>
-          <c:min val="0"/>
+          <c:max val="1000.0"/>
+          <c:min val="0.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -937,8 +951,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.29323901447802897"/>
-              <c:y val="0.91884753907156846"/>
+              <c:x val="0.293239014478029"/>
+              <c:y val="0.918847539071569"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -949,6 +963,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -978,20 +1009,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158078464"/>
-        <c:crossesAt val="-360"/>
+        <c:crossAx val="738071568"/>
+        <c:crossesAt val="-360.0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="250"/>
+        <c:majorUnit val="250.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="158078464"/>
+        <c:axId val="738071568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="4"/>
-          <c:min val="-4"/>
+          <c:max val="4.0"/>
+          <c:min val="-4.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1061,6 +1092,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -1090,13 +1138,13 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="156949888"/>
+        <c:crossAx val="738066160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="1"/>
+        <c:majorUnit val="1.0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1129,7 +1177,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1143,7 +1191,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1161,10 +1209,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.1563960714588096"/>
-          <c:y val="0.10979173639709001"/>
-          <c:w val="0.66648158496316989"/>
-          <c:h val="0.70963948710729141"/>
+          <c:x val="0.15639607145881"/>
+          <c:y val="0.10979173639709"/>
+          <c:w val="0.66648158496317"/>
+          <c:h val="0.709639487107291"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1211,217 +1259,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>445</c:v>
+                  <c:v>445.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>410</c:v>
+                  <c:v>410.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>301</c:v>
+                  <c:v>301.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>241</c:v>
+                  <c:v>241.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>375</c:v>
+                  <c:v>375.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>190</c:v>
+                  <c:v>190.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>202</c:v>
+                  <c:v>202.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>215</c:v>
+                  <c:v>215.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>445</c:v>
+                  <c:v>445.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>540</c:v>
+                  <c:v>540.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>626</c:v>
+                  <c:v>626.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>594</c:v>
+                  <c:v>594.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>506</c:v>
+                  <c:v>506.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>729</c:v>
+                  <c:v>729.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>423</c:v>
+                  <c:v>423.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>268</c:v>
+                  <c:v>268.0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>448</c:v>
+                  <c:v>448.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>119</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>147</c:v>
+                  <c:v>147.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>119</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>119</c:v>
+                  <c:v>119.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>361</c:v>
+                  <c:v>361.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>722</c:v>
+                  <c:v>722.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>850</c:v>
+                  <c:v>850.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>891</c:v>
+                  <c:v>891.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>326</c:v>
+                  <c:v>326.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>280</c:v>
+                  <c:v>280.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>683</c:v>
+                  <c:v>683.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>370</c:v>
+                  <c:v>370.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>380</c:v>
+                  <c:v>380.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>449</c:v>
+                  <c:v>449.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>994</c:v>
+                  <c:v>994.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1042</c:v>
+                  <c:v>1042.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1240</c:v>
+                  <c:v>1240.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>988</c:v>
+                  <c:v>988.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>954</c:v>
+                  <c:v>954.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>770</c:v>
+                  <c:v>770.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>982</c:v>
+                  <c:v>982.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>1274</c:v>
+                  <c:v>1274.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1217</c:v>
+                  <c:v>1217.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1283</c:v>
+                  <c:v>1283.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>212</c:v>
+                  <c:v>212.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>604</c:v>
+                  <c:v>604.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>580</c:v>
+                  <c:v>580.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>515</c:v>
+                  <c:v>515.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1002</c:v>
+                  <c:v>1002.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1210</c:v>
+                  <c:v>1210.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1256</c:v>
+                  <c:v>1256.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>430</c:v>
+                  <c:v>430.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>511</c:v>
+                  <c:v>511.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1166</c:v>
+                  <c:v>1166.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1173</c:v>
+                  <c:v>1173.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1072</c:v>
+                  <c:v>1072.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1115</c:v>
+                  <c:v>1115.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1193</c:v>
+                  <c:v>1193.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>567</c:v>
+                  <c:v>567.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1040</c:v>
+                  <c:v>1040.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1056</c:v>
+                  <c:v>1056.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1117</c:v>
+                  <c:v>1117.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1115</c:v>
+                  <c:v>1115.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1012</c:v>
+                  <c:v>1012.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1164</c:v>
+                  <c:v>1164.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1093</c:v>
+                  <c:v>1093.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1056</c:v>
+                  <c:v>1056.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1115</c:v>
+                  <c:v>1115.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>683</c:v>
+                  <c:v>683.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1196</c:v>
+                  <c:v>1196.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1204</c:v>
+                  <c:v>1204.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1241</c:v>
+                  <c:v>1241.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>872</c:v>
+                  <c:v>872.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1115</c:v>
+                  <c:v>1115.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1433,46 +1481,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>-31.411999999999999</c:v>
+                  <c:v>-31.412</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>-30.849</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-31.016999999999999</c:v>
+                  <c:v>-31.017</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-32.098999999999997</c:v>
+                  <c:v>-32.099</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>-31.166</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-30.856000000000002</c:v>
+                  <c:v>-30.856</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>-31.53</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-30.696000000000002</c:v>
+                  <c:v>-30.696</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-32.085999999999999</c:v>
+                  <c:v>-32.086</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-31.300999999999998</c:v>
+                  <c:v>-31.301</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-31.408000000000001</c:v>
+                  <c:v>-31.408</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>-31.936</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-31.513999999999999</c:v>
+                  <c:v>-31.514</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-31.123999999999999</c:v>
+                  <c:v>-31.124</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>-30.372</c:v>
@@ -1487,22 +1535,22 @@
                   <c:v>-30.51</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-30.379000000000001</c:v>
+                  <c:v>-30.379</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-30.591999999999999</c:v>
+                  <c:v>-30.592</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>-30.448</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-30.568999999999999</c:v>
+                  <c:v>-30.569</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-30.911000000000001</c:v>
+                  <c:v>-30.911</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-31.251000000000001</c:v>
+                  <c:v>-31.251</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>-31.186</c:v>
@@ -1511,37 +1559,37 @@
                   <c:v>-30.709</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-29.983000000000001</c:v>
+                  <c:v>-29.983</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>-30.45</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-30.263000000000002</c:v>
+                  <c:v>-30.263</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-30.053999999999998</c:v>
+                  <c:v>-30.054</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-30.079000000000001</c:v>
+                  <c:v>-30.079</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-31.202000000000002</c:v>
+                  <c:v>-31.202</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-30.518999999999998</c:v>
+                  <c:v>-30.519</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-31.231999999999999</c:v>
+                  <c:v>-31.232</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-31.219000000000001</c:v>
+                  <c:v>-31.219</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>-31.49</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-30.885999999999999</c:v>
+                  <c:v>-30.886</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>-31.878</c:v>
@@ -1553,67 +1601,67 @@
                   <c:v>-31.084</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-31.370999999999999</c:v>
+                  <c:v>-31.371</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-30.806999999999999</c:v>
+                  <c:v>-30.807</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-31.065000000000001</c:v>
+                  <c:v>-31.065</c:v>
                 </c:pt>
                 <c:pt idx="43">
                   <c:v>-30.741</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-31.385999999999999</c:v>
+                  <c:v>-31.386</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-31.234999999999999</c:v>
+                  <c:v>-31.235</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-31.486000000000001</c:v>
+                  <c:v>-31.486</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-31.405000000000001</c:v>
+                  <c:v>-31.405</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-31.332000000000001</c:v>
+                  <c:v>-31.332</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-30.957999999999998</c:v>
+                  <c:v>-30.958</c:v>
                 </c:pt>
                 <c:pt idx="50">
                   <c:v>-30.87</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-31.265000000000001</c:v>
+                  <c:v>-31.265</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-31.379000000000001</c:v>
+                  <c:v>-31.379</c:v>
                 </c:pt>
                 <c:pt idx="53">
                   <c:v>-31.366</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>-31.521999999999998</c:v>
+                  <c:v>-31.522</c:v>
                 </c:pt>
                 <c:pt idx="55">
                   <c:v>-31.282</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>-31.864000000000001</c:v>
+                  <c:v>-31.864</c:v>
                 </c:pt>
                 <c:pt idx="57">
                   <c:v>-31.529</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>-31.393000000000001</c:v>
+                  <c:v>-31.393</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>-31.512</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>-31.425000000000001</c:v>
+                  <c:v>-31.425</c:v>
                 </c:pt>
                 <c:pt idx="61">
                   <c:v>-31.47</c:v>
@@ -1622,25 +1670,25 @@
                   <c:v>-31.474</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>-30.908000000000001</c:v>
+                  <c:v>-30.908</c:v>
                 </c:pt>
                 <c:pt idx="64">
                   <c:v>-31.42</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>-31.106999999999999</c:v>
+                  <c:v>-31.107</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>-31.931000000000001</c:v>
+                  <c:v>-31.931</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>-31.704999999999998</c:v>
+                  <c:v>-31.705</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>-31.489000000000001</c:v>
+                  <c:v>-31.489</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>-31.015000000000001</c:v>
+                  <c:v>-31.015</c:v>
                 </c:pt>
                 <c:pt idx="70">
                   <c:v>-30.78</c:v>
@@ -1672,10 +1720,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2500</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1687,10 +1735,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-30.913492366503768</c:v>
+                  <c:v>-30.91349236650377</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-30.913492366503768</c:v>
+                  <c:v>-30.91349236650377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1720,10 +1768,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2500</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1735,10 +1783,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-31.413492366503768</c:v>
+                  <c:v>-31.41349236650377</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-31.413492366503768</c:v>
+                  <c:v>-31.41349236650377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,10 +1816,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2500</c:v>
+                  <c:v>2500.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1783,10 +1831,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-30.413492366503768</c:v>
+                  <c:v>-30.41349236650377</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-30.413492366503768</c:v>
+                  <c:v>-30.41349236650377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1801,14 +1849,14 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="158113152"/>
-        <c:axId val="158119424"/>
+        <c:axId val="737749760"/>
+        <c:axId val="737740368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="158113152"/>
+        <c:axId val="737749760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1500"/>
+          <c:max val="1500.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1843,8 +1891,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.29323901447802897"/>
-              <c:y val="0.91884753907156846"/>
+              <c:x val="0.293239014478029"/>
+              <c:y val="0.918847539071569"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1855,6 +1903,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -1884,20 +1949,20 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158119424"/>
-        <c:crossesAt val="-360"/>
+        <c:crossAx val="737740368"/>
+        <c:crossesAt val="-360.0"/>
         <c:crossBetween val="midCat"/>
-        <c:majorUnit val="500"/>
+        <c:majorUnit val="500.0"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="158119424"/>
+        <c:axId val="737740368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="-28"/>
-          <c:min val="-35"/>
+          <c:max val="-28.0"/>
+          <c:min val="-35.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1967,6 +2032,23 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -1996,10 +2078,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="158113152"/>
+        <c:crossAx val="737749760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2034,7 +2116,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3518,7 +3600,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3528,16 +3610,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S33" sqref="S33:U40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="16" max="16" width="11.42578125" style="2"/>
+    <col min="16" max="16" width="13" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="33.75" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:26" ht="34" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
@@ -3545,12 +3627,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="F3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="E4" t="s">
         <v>11</v>
       </c>
@@ -3558,7 +3640,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>0</v>
       </c>
@@ -3587,7 +3669,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>0</v>
       </c>
@@ -3623,7 +3705,7 @@
         <v>0.5673905025308188</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>0</v>
       </c>
@@ -3644,7 +3726,7 @@
         <v>-1.1971764705882353</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
         <v>0</v>
       </c>
@@ -3665,7 +3747,7 @@
         <v>-1.1491764705882352</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
         <v>0</v>
       </c>
@@ -3676,7 +3758,7 @@
         <v>-0.185</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
         <v>0</v>
       </c>
@@ -3720,7 +3802,7 @@
         <v>0.16182352941176492</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
         <v>0</v>
       </c>
@@ -3753,7 +3835,7 @@
         <v>0.49882352941176467</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>43040</v>
       </c>
@@ -3786,7 +3868,7 @@
         <v>0.53382352941176481</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>43040</v>
       </c>
@@ -3797,7 +3879,7 @@
         <v>-0.33600000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D14">
         <v>43040</v>
       </c>
@@ -3821,7 +3903,7 @@
         <v>-0.18817647058823517</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D15">
         <v>43040</v>
       </c>
@@ -3832,7 +3914,7 @@
         <v>1.175</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D16">
         <v>43040</v>
       </c>
@@ -3856,7 +3938,7 @@
         <v>-0.47917647058823509</v>
       </c>
     </row>
-    <row r="17" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D17">
         <v>43040</v>
       </c>
@@ -3867,7 +3949,7 @@
         <v>0.32800000000000001</v>
       </c>
     </row>
-    <row r="18" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D18">
         <v>43040</v>
       </c>
@@ -3878,7 +3960,7 @@
         <v>0.91700000000000004</v>
       </c>
     </row>
-    <row r="19" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D19">
         <v>43040</v>
       </c>
@@ -3910,7 +3992,7 @@
         <v>-1.0751764705882352</v>
       </c>
     </row>
-    <row r="20" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D20">
         <v>43011</v>
       </c>
@@ -3931,7 +4013,7 @@
         <v>-0.66317647058823503</v>
       </c>
     </row>
-    <row r="21" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D21">
         <v>43011</v>
       </c>
@@ -3942,7 +4024,7 @@
         <v>0.60499999999999998</v>
       </c>
     </row>
-    <row r="22" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D22">
         <v>43011</v>
       </c>
@@ -3974,7 +4056,7 @@
         <v>0.40042352941176484</v>
       </c>
     </row>
-    <row r="23" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D23">
         <v>43011</v>
       </c>
@@ -3995,7 +4077,7 @@
         <v>-3.6176470588235032E-2</v>
       </c>
     </row>
-    <row r="24" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D24">
         <v>43011</v>
       </c>
@@ -4006,7 +4088,7 @@
         <v>0.47899999999999998</v>
       </c>
     </row>
-    <row r="25" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D25">
         <v>43011</v>
       </c>
@@ -4030,7 +4112,7 @@
         <v>3.0823529411764916E-2</v>
       </c>
     </row>
-    <row r="26" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D26">
         <v>43011</v>
       </c>
@@ -4041,7 +4123,7 @@
         <v>-0.26400000000000001</v>
       </c>
     </row>
-    <row r="27" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D27">
         <v>43011</v>
       </c>
@@ -4065,7 +4147,7 @@
         <v>-0.61917647058823522</v>
       </c>
     </row>
-    <row r="28" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D28">
         <v>43011</v>
       </c>
@@ -4076,7 +4158,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="29" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D29">
         <v>43011</v>
       </c>
@@ -4087,7 +4169,7 @@
         <v>1.3939999999999999</v>
       </c>
     </row>
-    <row r="30" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D30">
         <v>43011</v>
       </c>
@@ -4098,7 +4180,7 @@
         <v>1.512</v>
       </c>
     </row>
-    <row r="31" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D31">
         <v>43000</v>
       </c>
@@ -4109,7 +4191,7 @@
         <v>0.81699999999999995</v>
       </c>
     </row>
-    <row r="32" spans="4:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:24" x14ac:dyDescent="0.2">
       <c r="D32">
         <v>43000</v>
       </c>
@@ -4123,7 +4205,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
         <v>1</v>
       </c>
@@ -4143,7 +4225,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
         <v>1</v>
       </c>
@@ -4168,7 +4250,7 @@
         <v>0.21840634911406137</v>
       </c>
     </row>
-    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
         <v>1</v>
       </c>
@@ -4193,7 +4275,7 @@
         <v>0.20541746112084361</v>
       </c>
     </row>
-    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
         <v>1</v>
       </c>
@@ -4218,7 +4300,7 @@
         <v>0.5673905025308188</v>
       </c>
     </row>
-    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
         <v>1</v>
       </c>
@@ -4249,7 +4331,7 @@
         <v>0.5673905025308188</v>
       </c>
     </row>
-    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E38">
         <v>689</v>
       </c>
@@ -4283,7 +4365,7 @@
         <v>0.30872282066604523</v>
       </c>
     </row>
-    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E39">
         <v>635</v>
       </c>
@@ -4323,7 +4405,7 @@
         <v>0.5673905025308188</v>
       </c>
     </row>
-    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E40">
         <v>471</v>
       </c>
@@ -4345,7 +4427,7 @@
         <v>0.5673905025308188</v>
       </c>
     </row>
-    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E41">
         <v>293</v>
       </c>
@@ -4353,7 +4435,7 @@
         <v>0.44700000000000001</v>
       </c>
     </row>
-    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E42">
         <v>663</v>
       </c>
@@ -4361,7 +4443,7 @@
         <v>1.0840000000000001</v>
       </c>
     </row>
-    <row r="43" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E43">
         <v>586</v>
       </c>
@@ -4369,7 +4451,7 @@
         <v>0.97799999999999998</v>
       </c>
     </row>
-    <row r="44" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E44">
         <v>371</v>
       </c>
@@ -4377,7 +4459,7 @@
         <v>-0.191</v>
       </c>
     </row>
-    <row r="45" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E45">
         <v>284</v>
       </c>
@@ -4385,7 +4467,7 @@
         <v>0.247</v>
       </c>
     </row>
-    <row r="46" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E46">
         <v>412</v>
       </c>
@@ -4393,7 +4475,7 @@
         <v>0.245</v>
       </c>
     </row>
-    <row r="47" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E47">
         <v>148</v>
       </c>
@@ -4404,7 +4486,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:21" x14ac:dyDescent="0.2">
       <c r="E48">
         <v>167</v>
       </c>
@@ -4418,7 +4500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E49">
         <v>292</v>
       </c>
@@ -4432,7 +4514,7 @@
         <v>2.0019999999999998</v>
       </c>
     </row>
-    <row r="50" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E50">
         <v>504</v>
       </c>
@@ -4446,7 +4528,7 @@
         <v>1.958</v>
       </c>
     </row>
-    <row r="51" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E51">
         <v>347</v>
       </c>
@@ -4460,7 +4542,7 @@
         <v>2.0329999999999999</v>
       </c>
     </row>
-    <row r="52" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E52">
         <v>278</v>
       </c>
@@ -4474,7 +4556,7 @@
         <v>1.6819999999999999</v>
       </c>
     </row>
-    <row r="53" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E53">
         <v>449</v>
       </c>
@@ -4488,7 +4570,7 @@
         <v>2.1629999999999998</v>
       </c>
     </row>
-    <row r="54" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E54">
         <v>359</v>
       </c>
@@ -4502,7 +4584,7 @@
         <v>1.3320000000000001</v>
       </c>
     </row>
-    <row r="55" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E55">
         <v>338</v>
       </c>
@@ -4516,7 +4598,7 @@
         <v>1.9019999999999999</v>
       </c>
     </row>
-    <row r="56" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E56">
         <v>349</v>
       </c>
@@ -4533,7 +4615,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:13" x14ac:dyDescent="0.2">
       <c r="I57">
         <v>578</v>
       </c>
@@ -4544,7 +4626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:13" x14ac:dyDescent="0.2">
       <c r="I58">
         <v>508</v>
       </c>
@@ -4555,7 +4637,7 @@
         <v>2.1139999999999999</v>
       </c>
     </row>
-    <row r="59" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E59" t="s">
         <v>12</v>
       </c>
@@ -4570,7 +4652,7 @@
         <v>1.9359999999999999</v>
       </c>
     </row>
-    <row r="60" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
         <v>7</v>
       </c>
@@ -4585,7 +4667,7 @@
         <v>1.8540000000000001</v>
       </c>
     </row>
-    <row r="61" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:13" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
         <v>13</v>
       </c>
@@ -4600,7 +4682,7 @@
         <v>2.1989999999999998</v>
       </c>
     </row>
-    <row r="62" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:13" x14ac:dyDescent="0.2">
       <c r="I62">
         <v>241</v>
       </c>
@@ -4608,7 +4690,7 @@
         <v>1.88</v>
       </c>
     </row>
-    <row r="63" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:13" x14ac:dyDescent="0.2">
       <c r="I63">
         <v>533</v>
       </c>
@@ -4616,7 +4698,7 @@
         <v>3.0550000000000002</v>
       </c>
     </row>
-    <row r="64" spans="5:13" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:13" x14ac:dyDescent="0.2">
       <c r="I64">
         <v>397</v>
       </c>
@@ -4624,7 +4706,7 @@
         <v>2.7160000000000002</v>
       </c>
     </row>
-    <row r="65" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="4:10" x14ac:dyDescent="0.2">
       <c r="I65">
         <v>184</v>
       </c>
@@ -4632,7 +4714,7 @@
         <v>1.946</v>
       </c>
     </row>
-    <row r="67" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="4:10" x14ac:dyDescent="0.2">
       <c r="I67" t="s">
         <v>12</v>
       </c>
@@ -4641,7 +4723,7 @@
         <v>1.8981764705882351</v>
       </c>
     </row>
-    <row r="68" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="4:10" x14ac:dyDescent="0.2">
       <c r="I68" t="s">
         <v>7</v>
       </c>
@@ -4650,7 +4732,7 @@
         <v>0.50637143423752207</v>
       </c>
     </row>
-    <row r="69" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="4:10" x14ac:dyDescent="0.2">
       <c r="I69" t="s">
         <v>13</v>
       </c>
@@ -4659,7 +4741,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D76" t="s">
         <v>16</v>
       </c>
@@ -4667,7 +4749,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D77">
         <v>445</v>
       </c>
@@ -4675,7 +4757,7 @@
         <v>-31.411999999999999</v>
       </c>
     </row>
-    <row r="78" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D78">
         <v>410</v>
       </c>
@@ -4683,7 +4765,7 @@
         <v>-30.849</v>
       </c>
     </row>
-    <row r="79" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D79">
         <v>301</v>
       </c>
@@ -4691,7 +4773,7 @@
         <v>-31.016999999999999</v>
       </c>
     </row>
-    <row r="80" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D80">
         <v>241</v>
       </c>
@@ -4699,7 +4781,7 @@
         <v>-32.098999999999997</v>
       </c>
     </row>
-    <row r="81" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D81">
         <v>375</v>
       </c>
@@ -4707,7 +4789,7 @@
         <v>-31.166</v>
       </c>
     </row>
-    <row r="82" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D82">
         <v>190</v>
       </c>
@@ -4715,7 +4797,7 @@
         <v>-30.856000000000002</v>
       </c>
     </row>
-    <row r="83" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D83">
         <v>202</v>
       </c>
@@ -4723,7 +4805,7 @@
         <v>-31.53</v>
       </c>
     </row>
-    <row r="84" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D84">
         <v>215</v>
       </c>
@@ -4731,7 +4813,7 @@
         <v>-30.696000000000002</v>
       </c>
     </row>
-    <row r="85" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D85">
         <v>445</v>
       </c>
@@ -4739,7 +4821,7 @@
         <v>-32.085999999999999</v>
       </c>
     </row>
-    <row r="86" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D86">
         <v>540</v>
       </c>
@@ -4747,7 +4829,7 @@
         <v>-31.300999999999998</v>
       </c>
     </row>
-    <row r="87" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D87">
         <v>626</v>
       </c>
@@ -4755,7 +4837,7 @@
         <v>-31.408000000000001</v>
       </c>
     </row>
-    <row r="88" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D88">
         <v>594</v>
       </c>
@@ -4763,7 +4845,7 @@
         <v>-31.936</v>
       </c>
     </row>
-    <row r="89" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D89">
         <v>506</v>
       </c>
@@ -4771,7 +4853,7 @@
         <v>-31.513999999999999</v>
       </c>
     </row>
-    <row r="90" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D90">
         <v>729</v>
       </c>
@@ -4779,7 +4861,7 @@
         <v>-31.123999999999999</v>
       </c>
     </row>
-    <row r="91" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D91">
         <v>423</v>
       </c>
@@ -4787,7 +4869,7 @@
         <v>-30.372</v>
       </c>
     </row>
-    <row r="92" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D92">
         <v>268</v>
       </c>
@@ -4795,7 +4877,7 @@
         <v>-30.689</v>
       </c>
     </row>
-    <row r="93" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D93">
         <v>448</v>
       </c>
@@ -4803,7 +4885,7 @@
         <v>-30.436</v>
       </c>
     </row>
-    <row r="94" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D94">
         <v>119</v>
       </c>
@@ -4811,7 +4893,7 @@
         <v>-30.51</v>
       </c>
     </row>
-    <row r="95" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D95">
         <v>147</v>
       </c>
@@ -4819,7 +4901,7 @@
         <v>-30.379000000000001</v>
       </c>
     </row>
-    <row r="96" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D96">
         <v>119</v>
       </c>
@@ -4827,7 +4909,7 @@
         <v>-30.591999999999999</v>
       </c>
     </row>
-    <row r="97" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D97">
         <v>119</v>
       </c>
@@ -4835,7 +4917,7 @@
         <v>-30.448</v>
       </c>
     </row>
-    <row r="98" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D98">
         <v>361</v>
       </c>
@@ -4843,7 +4925,7 @@
         <v>-30.568999999999999</v>
       </c>
     </row>
-    <row r="99" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D99">
         <v>722</v>
       </c>
@@ -4851,7 +4933,7 @@
         <v>-30.911000000000001</v>
       </c>
     </row>
-    <row r="100" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D100">
         <v>850</v>
       </c>
@@ -4859,7 +4941,7 @@
         <v>-31.251000000000001</v>
       </c>
     </row>
-    <row r="101" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D101">
         <v>891</v>
       </c>
@@ -4867,7 +4949,7 @@
         <v>-31.186</v>
       </c>
     </row>
-    <row r="102" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D102">
         <v>326</v>
       </c>
@@ -4875,7 +4957,7 @@
         <v>-30.709</v>
       </c>
     </row>
-    <row r="103" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D103">
         <v>280</v>
       </c>
@@ -4883,7 +4965,7 @@
         <v>-29.983000000000001</v>
       </c>
     </row>
-    <row r="104" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D104">
         <v>683</v>
       </c>
@@ -4891,7 +4973,7 @@
         <v>-30.45</v>
       </c>
     </row>
-    <row r="105" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D105">
         <v>370</v>
       </c>
@@ -4899,7 +4981,7 @@
         <v>-30.263000000000002</v>
       </c>
     </row>
-    <row r="106" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D106">
         <v>380</v>
       </c>
@@ -4907,7 +4989,7 @@
         <v>-30.053999999999998</v>
       </c>
     </row>
-    <row r="107" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D107">
         <v>449</v>
       </c>
@@ -4915,7 +4997,7 @@
         <v>-30.079000000000001</v>
       </c>
     </row>
-    <row r="108" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D108">
         <v>994</v>
       </c>
@@ -4923,7 +5005,7 @@
         <v>-31.202000000000002</v>
       </c>
     </row>
-    <row r="109" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D109">
         <v>1042</v>
       </c>
@@ -4931,7 +5013,7 @@
         <v>-30.518999999999998</v>
       </c>
     </row>
-    <row r="110" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D110">
         <v>1240</v>
       </c>
@@ -4939,7 +5021,7 @@
         <v>-31.231999999999999</v>
       </c>
     </row>
-    <row r="111" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D111">
         <v>988</v>
       </c>
@@ -4947,7 +5029,7 @@
         <v>-31.219000000000001</v>
       </c>
     </row>
-    <row r="112" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D112">
         <v>954</v>
       </c>
@@ -4955,7 +5037,7 @@
         <v>-31.49</v>
       </c>
     </row>
-    <row r="113" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="113" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D113">
         <v>770</v>
       </c>
@@ -4963,7 +5045,7 @@
         <v>-30.885999999999999</v>
       </c>
     </row>
-    <row r="114" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D114">
         <v>982</v>
       </c>
@@ -4971,7 +5053,7 @@
         <v>-31.878</v>
       </c>
     </row>
-    <row r="115" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D115">
         <v>1274</v>
       </c>
@@ -4979,7 +5061,7 @@
         <v>-31.48</v>
       </c>
     </row>
-    <row r="116" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D116">
         <v>1217</v>
       </c>
@@ -4987,7 +5069,7 @@
         <v>-31.084</v>
       </c>
     </row>
-    <row r="117" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="117" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D117">
         <v>1283</v>
       </c>
@@ -4995,7 +5077,7 @@
         <v>-31.370999999999999</v>
       </c>
     </row>
-    <row r="118" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="118" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D118">
         <v>212</v>
       </c>
@@ -5003,7 +5085,7 @@
         <v>-30.806999999999999</v>
       </c>
     </row>
-    <row r="119" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D119">
         <v>604</v>
       </c>
@@ -5014,7 +5096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D120">
         <v>580</v>
       </c>
@@ -5034,7 +5116,7 @@
         <v>-30.413492366503768</v>
       </c>
     </row>
-    <row r="121" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="121" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D121">
         <v>515</v>
       </c>
@@ -5054,7 +5136,7 @@
         <v>-30.413492366503768</v>
       </c>
     </row>
-    <row r="122" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="122" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D122">
         <v>1002</v>
       </c>
@@ -5062,7 +5144,7 @@
         <v>-31.234999999999999</v>
       </c>
     </row>
-    <row r="123" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="123" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D123">
         <v>1210</v>
       </c>
@@ -5070,7 +5152,7 @@
         <v>-31.486000000000001</v>
       </c>
     </row>
-    <row r="124" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D124">
         <v>1256</v>
       </c>
@@ -5078,7 +5160,7 @@
         <v>-31.405000000000001</v>
       </c>
     </row>
-    <row r="125" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D125">
         <v>430</v>
       </c>
@@ -5086,7 +5168,7 @@
         <v>-31.332000000000001</v>
       </c>
     </row>
-    <row r="126" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="126" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D126">
         <v>511</v>
       </c>
@@ -5094,7 +5176,7 @@
         <v>-30.957999999999998</v>
       </c>
     </row>
-    <row r="127" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D127">
         <v>1166</v>
       </c>
@@ -5102,7 +5184,7 @@
         <v>-30.87</v>
       </c>
     </row>
-    <row r="128" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D128">
         <v>1173</v>
       </c>
@@ -5110,7 +5192,7 @@
         <v>-31.265000000000001</v>
       </c>
     </row>
-    <row r="129" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D129">
         <v>1072</v>
       </c>
@@ -5118,7 +5200,7 @@
         <v>-31.379000000000001</v>
       </c>
     </row>
-    <row r="130" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D130">
         <v>1115</v>
       </c>
@@ -5126,7 +5208,7 @@
         <v>-31.366</v>
       </c>
     </row>
-    <row r="131" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D131">
         <v>1193</v>
       </c>
@@ -5134,7 +5216,7 @@
         <v>-31.521999999999998</v>
       </c>
     </row>
-    <row r="132" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D132">
         <v>567</v>
       </c>
@@ -5142,7 +5224,7 @@
         <v>-31.282</v>
       </c>
     </row>
-    <row r="133" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D133">
         <v>1040</v>
       </c>
@@ -5150,7 +5232,7 @@
         <v>-31.864000000000001</v>
       </c>
     </row>
-    <row r="134" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D134">
         <v>1056</v>
       </c>
@@ -5158,7 +5240,7 @@
         <v>-31.529</v>
       </c>
     </row>
-    <row r="135" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D135">
         <v>1117</v>
       </c>
@@ -5166,7 +5248,7 @@
         <v>-31.393000000000001</v>
       </c>
     </row>
-    <row r="136" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D136">
         <v>1115</v>
       </c>
@@ -5174,7 +5256,7 @@
         <v>-31.512</v>
       </c>
     </row>
-    <row r="137" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D137">
         <v>1012</v>
       </c>
@@ -5182,7 +5264,7 @@
         <v>-31.425000000000001</v>
       </c>
     </row>
-    <row r="138" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D138">
         <v>1164</v>
       </c>
@@ -5190,7 +5272,7 @@
         <v>-31.47</v>
       </c>
     </row>
-    <row r="139" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D139">
         <v>1093</v>
       </c>
@@ -5198,7 +5280,7 @@
         <v>-31.474</v>
       </c>
     </row>
-    <row r="140" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D140">
         <v>1056</v>
       </c>
@@ -5206,7 +5288,7 @@
         <v>-30.908000000000001</v>
       </c>
     </row>
-    <row r="141" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D141">
         <v>1115</v>
       </c>
@@ -5214,7 +5296,7 @@
         <v>-31.42</v>
       </c>
     </row>
-    <row r="142" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="142" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D142">
         <v>683</v>
       </c>
@@ -5222,7 +5304,7 @@
         <v>-31.106999999999999</v>
       </c>
     </row>
-    <row r="143" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="143" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D143">
         <v>1196</v>
       </c>
@@ -5230,7 +5312,7 @@
         <v>-31.931000000000001</v>
       </c>
     </row>
-    <row r="144" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="144" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D144">
         <v>1204</v>
       </c>
@@ -5238,7 +5320,7 @@
         <v>-31.704999999999998</v>
       </c>
     </row>
-    <row r="145" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="145" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D145">
         <v>1241</v>
       </c>
@@ -5246,7 +5328,7 @@
         <v>-31.489000000000001</v>
       </c>
     </row>
-    <row r="146" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="146" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D146">
         <v>872</v>
       </c>
@@ -5254,7 +5336,7 @@
         <v>-31.015000000000001</v>
       </c>
     </row>
-    <row r="147" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="147" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D147">
         <v>1115</v>
       </c>
@@ -5262,7 +5344,7 @@
         <v>-30.78</v>
       </c>
     </row>
-    <row r="150" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="150" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D150" t="s">
         <v>41</v>
       </c>
@@ -5271,7 +5353,7 @@
         <v>-31.117704225352114</v>
       </c>
     </row>
-    <row r="151" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="151" spans="4:5" x14ac:dyDescent="0.2">
       <c r="D151" t="s">
         <v>7</v>
       </c>
@@ -5295,19 +5377,19 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C1" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>29</v>
       </c>
@@ -5315,7 +5397,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -5326,22 +5408,22 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C9" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="D10" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F11" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -5349,7 +5431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>34</v>
       </c>

</xml_diff>